<commit_message>
fix: :zap: last version
</commit_message>
<xml_diff>
--- a/inventory_products.xlsx
+++ b/inventory_products.xlsx
@@ -425,7 +425,7 @@
         <v>1252579719</v>
       </c>
       <c r="F2" s="9" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G2" s="10" t="n">
         <v>3</v>
@@ -434,14 +434,14 @@
         <v>0</v>
       </c>
       <c r="I2" s="12" t="n">
-        <v>12098005</v>
+        <v>12763618</v>
       </c>
       <c r="J2" s="13" t="n">
-        <v>12098005</v>
+        <v>13315700</v>
       </c>
       <c r="K2" s="14" t="inlineStr">
         <is>
-          <t>بله</t>
+          <t>خیر</t>
         </is>
       </c>
       <c r="L2" s="15" t="n">
@@ -461,7 +461,7 @@
       <c r="T2" s="23"/>
       <c r="U2" s="24" t="inlineStr">
         <is>
-          <t>eb9ef7e2d6d8</t>
+          <t>560dffbb71d7</t>
         </is>
       </c>
       <c r="V2" s="25"/>
@@ -501,10 +501,10 @@
         <v>0</v>
       </c>
       <c r="I3" s="12" t="n">
-        <v>12306591</v>
+        <v>12983681</v>
       </c>
       <c r="J3" s="13" t="n">
-        <v>12306591</v>
+        <v>12983681</v>
       </c>
       <c r="K3" s="14" t="inlineStr">
         <is>
@@ -528,7 +528,7 @@
       <c r="T3" s="23"/>
       <c r="U3" s="24" t="inlineStr">
         <is>
-          <t>fb9bef44275b</t>
+          <t>dd15d9a2e318</t>
         </is>
       </c>
       <c r="V3" s="25"/>
@@ -568,10 +568,10 @@
         <v>1</v>
       </c>
       <c r="I4" s="12" t="n">
-        <v>13017389</v>
+        <v>13733586</v>
       </c>
       <c r="J4" s="13" t="n">
-        <v>13017389</v>
+        <v>13733586</v>
       </c>
       <c r="K4" s="14" t="inlineStr">
         <is>
@@ -595,11 +595,13 @@
       <c r="T4" s="23"/>
       <c r="U4" s="24" t="inlineStr">
         <is>
-          <t>cd3c7a85e0a7</t>
+          <t>6dea89bb4663</t>
         </is>
       </c>
       <c r="V4" s="25"/>
-      <c r="W4" s="26"/>
+      <c r="W4" s="26" t="n">
+        <v>12908932</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="5">
       <c r="A5" s="4" t="inlineStr">
@@ -635,10 +637,10 @@
         <v>1</v>
       </c>
       <c r="I5" s="12" t="n">
-        <v>13253252</v>
+        <v>13982425</v>
       </c>
       <c r="J5" s="13" t="n">
-        <v>13253252</v>
+        <v>13982425</v>
       </c>
       <c r="K5" s="14" t="inlineStr">
         <is>
@@ -662,11 +664,13 @@
       <c r="T5" s="23"/>
       <c r="U5" s="24" t="inlineStr">
         <is>
-          <t>41af0b0daf9e</t>
+          <t>b4d8915d08e9</t>
         </is>
       </c>
       <c r="V5" s="25"/>
-      <c r="W5" s="26"/>
+      <c r="W5" s="26" t="n">
+        <v>13142829</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="6">
       <c r="A6" s="4" t="inlineStr">
@@ -702,10 +706,10 @@
         <v>1</v>
       </c>
       <c r="I6" s="12" t="n">
-        <v>11539635</v>
+        <v>12174528</v>
       </c>
       <c r="J6" s="13" t="n">
-        <v>11539635</v>
+        <v>12174528</v>
       </c>
       <c r="K6" s="14" t="inlineStr">
         <is>
@@ -729,7 +733,7 @@
       <c r="T6" s="23"/>
       <c r="U6" s="24" t="inlineStr">
         <is>
-          <t>ddeb0d65d796</t>
+          <t>b2052a9afc39</t>
         </is>
       </c>
       <c r="V6" s="25"/>
@@ -769,10 +773,10 @@
         <v>0</v>
       </c>
       <c r="I7" s="12" t="n">
-        <v>14105247</v>
+        <v>14881296</v>
       </c>
       <c r="J7" s="13" t="n">
-        <v>14105247</v>
+        <v>14881296</v>
       </c>
       <c r="K7" s="14" t="inlineStr">
         <is>
@@ -796,7 +800,7 @@
       <c r="T7" s="23"/>
       <c r="U7" s="24" t="inlineStr">
         <is>
-          <t>781e7b52749a</t>
+          <t>a578315a9058</t>
         </is>
       </c>
       <c r="V7" s="25"/>
@@ -836,18 +840,16 @@
         <v>0</v>
       </c>
       <c r="I8" s="12" t="n">
-        <v>8515134</v>
-      </c>
-      <c r="J8" s="13" t="n">
-        <v>8515134</v>
-      </c>
+        <v>8983624</v>
+      </c>
+      <c r="J8" s="13"/>
       <c r="K8" s="14" t="inlineStr">
         <is>
-          <t>بله</t>
+          <t>خیر</t>
         </is>
       </c>
       <c r="L8" s="15" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M8" s="16" t="n">
         <v>0</v>
@@ -863,11 +865,13 @@
       <c r="T8" s="23"/>
       <c r="U8" s="24" t="inlineStr">
         <is>
-          <t>957b26826790</t>
+          <t>87057c30d818</t>
         </is>
       </c>
       <c r="V8" s="25"/>
-      <c r="W8" s="26"/>
+      <c r="W8" s="26" t="n">
+        <v>8444188</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="9">
       <c r="A9" s="4" t="inlineStr">
@@ -903,10 +907,10 @@
         <v>1</v>
       </c>
       <c r="I9" s="12" t="n">
-        <v>10220728</v>
+        <v>10783057</v>
       </c>
       <c r="J9" s="13" t="n">
-        <v>10220728</v>
+        <v>10783057</v>
       </c>
       <c r="K9" s="14" t="inlineStr">
         <is>
@@ -930,7 +934,7 @@
       <c r="T9" s="23"/>
       <c r="U9" s="24" t="inlineStr">
         <is>
-          <t>bd6ee062e862</t>
+          <t>dac685ad246b</t>
         </is>
       </c>
       <c r="V9" s="25"/>

</xml_diff>

<commit_message>
fix: update SNAPP_TOKEN in .env file
</commit_message>
<xml_diff>
--- a/inventory_products.xlsx
+++ b/inventory_products.xlsx
@@ -434,7 +434,7 @@
         <v>0</v>
       </c>
       <c r="I2" s="12" t="n">
-        <v>4950000</v>
+        <v>12239471</v>
       </c>
       <c r="J2" s="13" t="n">
         <v>13413000</v>
@@ -461,7 +461,7 @@
       <c r="T2" s="23"/>
       <c r="U2" s="24" t="inlineStr">
         <is>
-          <t>1282a5d4c8a2</t>
+          <t>c9db631f8c37</t>
         </is>
       </c>
       <c r="V2" s="25"/>
@@ -501,10 +501,10 @@
         <v>0</v>
       </c>
       <c r="I3" s="12" t="n">
-        <v>12983681</v>
+        <v>12450497</v>
       </c>
       <c r="J3" s="13" t="n">
-        <v>12983681</v>
+        <v>12450497</v>
       </c>
       <c r="K3" s="14" t="inlineStr">
         <is>
@@ -528,7 +528,7 @@
       <c r="T3" s="23"/>
       <c r="U3" s="24" t="inlineStr">
         <is>
-          <t>dd15d9a2e318</t>
+          <t>61428cd16d16</t>
         </is>
       </c>
       <c r="V3" s="25"/>
@@ -568,10 +568,10 @@
         <v>1</v>
       </c>
       <c r="I4" s="12" t="n">
-        <v>13733586</v>
+        <v>13169606</v>
       </c>
       <c r="J4" s="13" t="n">
-        <v>13733586</v>
+        <v>13169606</v>
       </c>
       <c r="K4" s="14" t="inlineStr">
         <is>
@@ -595,7 +595,7 @@
       <c r="T4" s="23"/>
       <c r="U4" s="24" t="inlineStr">
         <is>
-          <t>6dea89bb4663</t>
+          <t>a6a714f70d53</t>
         </is>
       </c>
       <c r="V4" s="25"/>
@@ -637,10 +637,10 @@
         <v>1</v>
       </c>
       <c r="I5" s="12" t="n">
-        <v>13982425</v>
+        <v>13408227</v>
       </c>
       <c r="J5" s="13" t="n">
-        <v>13982425</v>
+        <v>13408227</v>
       </c>
       <c r="K5" s="14" t="inlineStr">
         <is>
@@ -664,7 +664,7 @@
       <c r="T5" s="23"/>
       <c r="U5" s="24" t="inlineStr">
         <is>
-          <t>b4d8915d08e9</t>
+          <t>d05f058d66d3</t>
         </is>
       </c>
       <c r="V5" s="25"/>
@@ -706,10 +706,10 @@
         <v>1</v>
       </c>
       <c r="I6" s="12" t="n">
-        <v>12174528</v>
+        <v>11674573</v>
       </c>
       <c r="J6" s="13" t="n">
-        <v>12174528</v>
+        <v>11674573</v>
       </c>
       <c r="K6" s="14" t="inlineStr">
         <is>
@@ -733,7 +733,7 @@
       <c r="T6" s="23"/>
       <c r="U6" s="24" t="inlineStr">
         <is>
-          <t>b2052a9afc39</t>
+          <t>164a286afaa7</t>
         </is>
       </c>
       <c r="V6" s="25"/>
@@ -773,10 +773,10 @@
         <v>0</v>
       </c>
       <c r="I7" s="12" t="n">
-        <v>14881296</v>
+        <v>14270185</v>
       </c>
       <c r="J7" s="13" t="n">
-        <v>14881296</v>
+        <v>14270185</v>
       </c>
       <c r="K7" s="14" t="inlineStr">
         <is>
@@ -800,7 +800,7 @@
       <c r="T7" s="23"/>
       <c r="U7" s="24" t="inlineStr">
         <is>
-          <t>a578315a9058</t>
+          <t>8c5312a5e111</t>
         </is>
       </c>
       <c r="V7" s="25"/>
@@ -840,16 +840,18 @@
         <v>0</v>
       </c>
       <c r="I8" s="12" t="n">
-        <v>4950000</v>
-      </c>
-      <c r="J8" s="13"/>
+        <v>8614705</v>
+      </c>
+      <c r="J8" s="13" t="n">
+        <v>8614705</v>
+      </c>
       <c r="K8" s="14" t="inlineStr">
         <is>
-          <t>خیر</t>
+          <t>بله</t>
         </is>
       </c>
       <c r="L8" s="15" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M8" s="16" t="n">
         <v>0</v>
@@ -865,7 +867,7 @@
       <c r="T8" s="23"/>
       <c r="U8" s="24" t="inlineStr">
         <is>
-          <t>f40bdfd14ec2</t>
+          <t>3c989061899b</t>
         </is>
       </c>
       <c r="V8" s="25"/>
@@ -907,10 +909,10 @@
         <v>1</v>
       </c>
       <c r="I9" s="12" t="n">
-        <v>4950000</v>
+        <v>10340243</v>
       </c>
       <c r="J9" s="13" t="n">
-        <v>4950000</v>
+        <v>10340243</v>
       </c>
       <c r="K9" s="14" t="inlineStr">
         <is>
@@ -934,11 +936,13 @@
       <c r="T9" s="23"/>
       <c r="U9" s="24" t="inlineStr">
         <is>
-          <t>420fcb6c779b</t>
+          <t>dc37d0e519e4</t>
         </is>
       </c>
       <c r="V9" s="25"/>
-      <c r="W9" s="26"/>
+      <c r="W9" s="26" t="n">
+        <v>4950000</v>
+      </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>

<commit_message>
fix: update SNAPP_TOKEN and handle error response in updatePrice.js
</commit_message>
<xml_diff>
--- a/inventory_products.xlsx
+++ b/inventory_products.xlsx
@@ -408,7 +408,7 @@
       </c>
       <c r="B2" s="5" t="inlineStr">
         <is>
-          <t>گردنبند زنانه</t>
+          <t>گردنبند طلا زنانه</t>
         </is>
       </c>
       <c r="C2" s="6" t="inlineStr">
@@ -434,10 +434,10 @@
         <v>0</v>
       </c>
       <c r="I2" s="12" t="n">
-        <v>12239471</v>
+        <v>12073284</v>
       </c>
       <c r="J2" s="13" t="n">
-        <v>13413000</v>
+        <v>13901400</v>
       </c>
       <c r="K2" s="14" t="inlineStr">
         <is>
@@ -461,7 +461,7 @@
       <c r="T2" s="23"/>
       <c r="U2" s="24" t="inlineStr">
         <is>
-          <t>c9db631f8c37</t>
+          <t>3d0df742b5b4</t>
         </is>
       </c>
       <c r="V2" s="25"/>
@@ -492,7 +492,7 @@
         <v>1017924412</v>
       </c>
       <c r="F3" s="9" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G3" s="10" t="n">
         <v>3</v>
@@ -501,14 +501,12 @@
         <v>0</v>
       </c>
       <c r="I3" s="12" t="n">
-        <v>12450497</v>
-      </c>
-      <c r="J3" s="13" t="n">
-        <v>12450497</v>
-      </c>
+        <v>12281444</v>
+      </c>
+      <c r="J3" s="13"/>
       <c r="K3" s="14" t="inlineStr">
         <is>
-          <t>بله</t>
+          <t>خیر</t>
         </is>
       </c>
       <c r="L3" s="15" t="n">
@@ -528,7 +526,7 @@
       <c r="T3" s="23"/>
       <c r="U3" s="24" t="inlineStr">
         <is>
-          <t>61428cd16d16</t>
+          <t>e6723b848790</t>
         </is>
       </c>
       <c r="V3" s="25"/>
@@ -559,7 +557,7 @@
         <v>984171003</v>
       </c>
       <c r="F4" s="9" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G4" s="10" t="n">
         <v>3</v>
@@ -568,14 +566,12 @@
         <v>1</v>
       </c>
       <c r="I4" s="12" t="n">
-        <v>13169606</v>
-      </c>
-      <c r="J4" s="13" t="n">
-        <v>13169606</v>
-      </c>
+        <v>12990789</v>
+      </c>
+      <c r="J4" s="13"/>
       <c r="K4" s="14" t="inlineStr">
         <is>
-          <t>بله</t>
+          <t>خیر</t>
         </is>
       </c>
       <c r="L4" s="15" t="n">
@@ -595,7 +591,7 @@
       <c r="T4" s="23"/>
       <c r="U4" s="24" t="inlineStr">
         <is>
-          <t>a6a714f70d53</t>
+          <t>f645dc1c02a6</t>
         </is>
       </c>
       <c r="V4" s="25"/>
@@ -628,7 +624,7 @@
         <v>1981168834</v>
       </c>
       <c r="F5" s="9" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G5" s="10" t="n">
         <v>1</v>
@@ -637,14 +633,12 @@
         <v>1</v>
       </c>
       <c r="I5" s="12" t="n">
-        <v>13408227</v>
-      </c>
-      <c r="J5" s="13" t="n">
-        <v>13408227</v>
-      </c>
+        <v>13226170</v>
+      </c>
+      <c r="J5" s="13"/>
       <c r="K5" s="14" t="inlineStr">
         <is>
-          <t>بله</t>
+          <t>خیر</t>
         </is>
       </c>
       <c r="L5" s="15" t="n">
@@ -664,7 +658,7 @@
       <c r="T5" s="23"/>
       <c r="U5" s="24" t="inlineStr">
         <is>
-          <t>d05f058d66d3</t>
+          <t>ee6ebc510dbb</t>
         </is>
       </c>
       <c r="V5" s="25"/>
@@ -697,7 +691,7 @@
         <v>76891083</v>
       </c>
       <c r="F6" s="9" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G6" s="10" t="n">
         <v>1</v>
@@ -706,14 +700,12 @@
         <v>1</v>
       </c>
       <c r="I6" s="12" t="n">
-        <v>11674573</v>
-      </c>
-      <c r="J6" s="13" t="n">
-        <v>11674573</v>
-      </c>
+        <v>11516055</v>
+      </c>
+      <c r="J6" s="13"/>
       <c r="K6" s="14" t="inlineStr">
         <is>
-          <t>بله</t>
+          <t>خیر</t>
         </is>
       </c>
       <c r="L6" s="15" t="n">
@@ -733,7 +725,7 @@
       <c r="T6" s="23"/>
       <c r="U6" s="24" t="inlineStr">
         <is>
-          <t>164a286afaa7</t>
+          <t>fac4c114bf4d</t>
         </is>
       </c>
       <c r="V6" s="25"/>
@@ -764,7 +756,7 @@
         <v>1337113337</v>
       </c>
       <c r="F7" s="9" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G7" s="10" t="n">
         <v>3</v>
@@ -773,14 +765,12 @@
         <v>0</v>
       </c>
       <c r="I7" s="12" t="n">
-        <v>14270185</v>
-      </c>
-      <c r="J7" s="13" t="n">
-        <v>14270185</v>
-      </c>
+        <v>14076424</v>
+      </c>
+      <c r="J7" s="13"/>
       <c r="K7" s="14" t="inlineStr">
         <is>
-          <t>بله</t>
+          <t>خیر</t>
         </is>
       </c>
       <c r="L7" s="15" t="n">
@@ -800,7 +790,7 @@
       <c r="T7" s="23"/>
       <c r="U7" s="24" t="inlineStr">
         <is>
-          <t>8c5312a5e111</t>
+          <t>1ffc27d247d8</t>
         </is>
       </c>
       <c r="V7" s="25"/>
@@ -831,7 +821,7 @@
         <v>269410027</v>
       </c>
       <c r="F8" s="9" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G8" s="10" t="n">
         <v>3</v>
@@ -840,14 +830,12 @@
         <v>0</v>
       </c>
       <c r="I8" s="12" t="n">
-        <v>8614705</v>
-      </c>
-      <c r="J8" s="13" t="n">
-        <v>8614705</v>
-      </c>
+        <v>8497734</v>
+      </c>
+      <c r="J8" s="13"/>
       <c r="K8" s="14" t="inlineStr">
         <is>
-          <t>بله</t>
+          <t>خیر</t>
         </is>
       </c>
       <c r="L8" s="15" t="n">
@@ -867,7 +855,7 @@
       <c r="T8" s="23"/>
       <c r="U8" s="24" t="inlineStr">
         <is>
-          <t>3c989061899b</t>
+          <t>dc5486bd1e10</t>
         </is>
       </c>
       <c r="V8" s="25"/>
@@ -900,7 +888,7 @@
         <v>1698323769</v>
       </c>
       <c r="F9" s="9" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G9" s="10" t="n">
         <v>3</v>
@@ -909,14 +897,12 @@
         <v>1</v>
       </c>
       <c r="I9" s="12" t="n">
-        <v>10340243</v>
-      </c>
-      <c r="J9" s="13" t="n">
-        <v>10340243</v>
-      </c>
+        <v>22200000</v>
+      </c>
+      <c r="J9" s="13"/>
       <c r="K9" s="14" t="inlineStr">
         <is>
-          <t>بله</t>
+          <t>خیر</t>
         </is>
       </c>
       <c r="L9" s="15" t="n">
@@ -936,7 +922,7 @@
       <c r="T9" s="23"/>
       <c r="U9" s="24" t="inlineStr">
         <is>
-          <t>dc37d0e519e4</t>
+          <t>889469343ae2</t>
         </is>
       </c>
       <c r="V9" s="25"/>

</xml_diff>